<commit_message>
added more graphs and bar charts
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,21 @@
           <t>Without PII</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Processing Time (s)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Processing Time per File (s)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cost per Million Tokens</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -454,6 +469,15 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -462,7 +486,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="C3" t="n">
+        <v>733</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7.33</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +505,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="C4" t="n">
+        <v>406</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4.06</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.18</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +524,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="C5" t="n">
+        <v>639</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6.39</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>